<commit_message>
mise à jour du bakclog
</commit_message>
<xml_diff>
--- a/gestion-projet/ProductBacklog.xlsx
+++ b/gestion-projet/ProductBacklog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sgobin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wsjs\stacktrace\gestion-projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{852D1FED-E8A4-4CD6-BB57-FE1927D5DA98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23021A10-1E9D-413E-9E87-FE58E19AD274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{1FDB83B7-599D-4D42-AA13-F5EE32DADB90}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="49">
-  <si>
-    <t>PRODUCT BACKLOG ENISSUE</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="57">
   <si>
     <t>Priorité</t>
   </si>
@@ -86,21 +83,9 @@
     <t>US001</t>
   </si>
   <si>
-    <t>Création de la page d'accueil statique qui permettra de lister toutes les issues (messages) - Les issues sont gérées dans un tableau d'issues dans app.js</t>
-  </si>
-  <si>
-    <t>Une issue/message est composée de : auteur / date-creation / titre / description / état (en-cours / résolu)</t>
-  </si>
-  <si>
     <t>US005</t>
   </si>
   <si>
-    <t>Ajouter une issue/message</t>
-  </si>
-  <si>
-    <t>En tant qu'utilisateur je peux saisir les informations d'une issue dans un formulaire et ajouter le message à la liste des messages</t>
-  </si>
-  <si>
     <t>US004</t>
   </si>
   <si>
@@ -113,42 +98,18 @@
     <t>US006</t>
   </si>
   <si>
-    <t xml:space="preserve">Supprimer un message </t>
-  </si>
-  <si>
-    <t>En tant qu'utilisateur je peux cliquer sur un lien "supprimer" qui supprime l'issue concernée</t>
-  </si>
-  <si>
     <t>US007</t>
   </si>
   <si>
-    <t>Modifier un message</t>
-  </si>
-  <si>
-    <t>En tant qu'utilisateur je peux charger une issue/message dans un formulaire pour modification et enregistrer la modification</t>
-  </si>
-  <si>
     <t>US008</t>
   </si>
   <si>
-    <t>Page détail d'une issue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">En tant qu'utilisateur je peux cliquer sur le titre d'une issue dans la page liste des issues et accéder au détail de l'issue </t>
-  </si>
-  <si>
     <t>V3</t>
   </si>
   <si>
-    <t>US009</t>
-  </si>
-  <si>
     <t>Gestion des réponses</t>
   </si>
   <si>
-    <t xml:space="preserve">Sur la page détail d'une issue, je peux ajouter, modifier ou supprimer une réponse à l'issue. </t>
-  </si>
-  <si>
     <t>US010</t>
   </si>
   <si>
@@ -183,6 +144,69 @@
   </si>
   <si>
     <t>Le titre est obligatoire et n'est pas blanc - la description fait plus de 3 caractères. Le traitement du formulaire doit protéger des injections XSS</t>
+  </si>
+  <si>
+    <t>PRODUCT BACKLOG ENticket</t>
+  </si>
+  <si>
+    <t>En tant qu'utilisateur je peux cliquer sur un lien "supprimer" qui supprime l'ticket concernée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En tant qu'utilisateur je peux cliquer sur le titre d'une ticket dans la page liste des tickets et accéder au détail de l'ticket </t>
+  </si>
+  <si>
+    <t>En tant qu'utilisateur je peux saisir les informations d'une ticket dans un formulaire et ajouter le ticket à la liste des tickets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supprimer un ticket </t>
+  </si>
+  <si>
+    <t>Modifier un ticket</t>
+  </si>
+  <si>
+    <t>En tant qu'utilisateur je peux charger une ticket/ticket dans un formulaire pour modification et enregistrer la modification</t>
+  </si>
+  <si>
+    <t>Ajouter une ticket</t>
+  </si>
+  <si>
+    <t>US014</t>
+  </si>
+  <si>
+    <t>US015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gestion de l'authentification </t>
+  </si>
+  <si>
+    <t>Chaque utilisateur a un login et mot de passe, ainsi qu'un rôle (Formateur ou élève)</t>
+  </si>
+  <si>
+    <t>V7</t>
+  </si>
+  <si>
+    <t>US016</t>
+  </si>
+  <si>
+    <t>Se déconnecter</t>
+  </si>
+  <si>
+    <t>US017</t>
+  </si>
+  <si>
+    <t>Seul l'auteur du ticket ou le formateur peut supprimer ou modifier un ticket.</t>
+  </si>
+  <si>
+    <t>Création de la page d'accueil  qui permettra de lister toutes les tickets - Les tickets sont gérés en mémoire dans un tableau de tickets dans app.js</t>
+  </si>
+  <si>
+    <t>Une ticket est composée de : auteur / date-creation / titre / description / état (ouvert / clos)</t>
+  </si>
+  <si>
+    <t>Page détail d'un ticket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sur la page détail d'une ticket, je peux ajouter, modifier ou supprimer une réponse à un ticket. </t>
   </si>
 </sst>
 </file>
@@ -227,18 +251,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -248,7 +266,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -306,7 +324,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -325,57 +343,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -713,435 +719,471 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52D07A81-0E55-45DE-A090-3CCE23AAB227}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="11.5546875" style="6"/>
-    <col min="3" max="3" width="78.33203125" customWidth="1"/>
+    <col min="3" max="3" width="84" customWidth="1"/>
     <col min="4" max="4" width="66.5546875" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" style="28" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="33.6" x14ac:dyDescent="0.65">
       <c r="C1" s="4" t="s">
-        <v>0</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="9"/>
+      <c r="F3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="17"/>
-      <c r="F3" s="25" t="s">
+      <c r="G3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="27" t="s">
+    </row>
+    <row r="4" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="16">
+        <v>1150</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="22"/>
+    </row>
+    <row r="5" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="16">
+        <v>1130</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="19"/>
+      <c r="E5" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="22"/>
+      <c r="I5" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="16">
+        <v>1100</v>
+      </c>
+      <c r="B6" s="17" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8">
-        <v>1150</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="11" t="s">
+      <c r="C6" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="F6" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="29"/>
-    </row>
-    <row r="5" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8">
-        <v>1130</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="18" t="s">
+      <c r="G6" s="22"/>
+    </row>
+    <row r="7" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="16">
+        <v>1000</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="29"/>
-      <c r="I5" s="16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="12">
-        <v>1100</v>
-      </c>
-      <c r="B6" s="13" t="s">
+      <c r="G7" s="22"/>
+    </row>
+    <row r="8" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="16">
+        <v>999</v>
+      </c>
+      <c r="B8" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="15" t="s">
+      <c r="C8" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="29"/>
-    </row>
-    <row r="7" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="21">
-        <v>1000</v>
-      </c>
-      <c r="B7" s="22" t="s">
+      <c r="D8" s="19"/>
+      <c r="E8" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="G8" s="22"/>
+    </row>
+    <row r="9" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="16">
+        <v>998</v>
+      </c>
+      <c r="B9" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="C9" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="22"/>
+    </row>
+    <row r="10" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="16">
+        <v>997</v>
+      </c>
+      <c r="B10" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="29"/>
-    </row>
-    <row r="8" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
-        <v>999</v>
-      </c>
-      <c r="B8" s="7" t="s">
+      <c r="C10" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="22"/>
+    </row>
+    <row r="11" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="16">
+        <v>995</v>
+      </c>
+      <c r="B11" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C11" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="29"/>
-    </row>
-    <row r="9" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
-        <v>998</v>
-      </c>
-      <c r="B9" s="7" t="s">
+      <c r="G11" s="22"/>
+    </row>
+    <row r="12" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="16">
+        <v>970</v>
+      </c>
+      <c r="B12" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C12" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D12" s="19"/>
+      <c r="E12" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="22"/>
+    </row>
+    <row r="13" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="16">
+        <v>960</v>
+      </c>
+      <c r="B13" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="20"/>
-      <c r="F9" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" s="29"/>
-    </row>
-    <row r="10" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
-        <v>997</v>
-      </c>
-      <c r="B10" s="7" t="s">
+      <c r="C13" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="22"/>
+    </row>
+    <row r="14" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="16">
+        <v>950</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="20"/>
-      <c r="F10" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="G10" s="29"/>
-    </row>
-    <row r="11" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
-        <v>995</v>
-      </c>
-      <c r="B11" s="7" t="s">
+      <c r="D14" s="19"/>
+      <c r="E14" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="20"/>
-      <c r="F11" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="29"/>
-    </row>
-    <row r="12" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
-        <v>970</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="G12" s="29"/>
-    </row>
-    <row r="13" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
-        <v>960</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E13" s="20"/>
-      <c r="F13" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="G13" s="29"/>
-    </row>
-    <row r="14" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
-        <v>950</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="G14" s="29"/>
+      <c r="G14" s="22"/>
     </row>
     <row r="15" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>940</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="D15" s="5"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="G15" s="29"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="15"/>
     </row>
     <row r="16" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>930</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" s="20"/>
-      <c r="F16" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="F16" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="15"/>
+    </row>
+    <row r="17" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>900</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="G16" s="29"/>
-    </row>
-    <row r="17" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="29"/>
+      <c r="C17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" s="10"/>
+      <c r="F17" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G17" s="15"/>
     </row>
     <row r="18" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="3"/>
+      <c r="A18" s="2">
+        <v>890</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="D18" s="5"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="29"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="15"/>
     </row>
     <row r="19" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="3"/>
+      <c r="A19" s="2">
+        <v>8880</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="D19" s="5"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="29"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="15"/>
     </row>
     <row r="20" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="7"/>
       <c r="C20" s="3"/>
       <c r="D20" s="5"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="29"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="15"/>
     </row>
     <row r="21" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="7"/>
       <c r="C21" s="3"/>
       <c r="D21" s="5"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="29"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="15"/>
     </row>
     <row r="22" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="7"/>
       <c r="C22" s="3"/>
       <c r="D22" s="5"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="29"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="15"/>
     </row>
     <row r="23" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="7"/>
       <c r="C23" s="3"/>
       <c r="D23" s="5"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="29"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="15"/>
     </row>
     <row r="24" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="7"/>
       <c r="C24" s="3"/>
       <c r="D24" s="5"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="29"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="15"/>
     </row>
     <row r="25" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" s="7"/>
       <c r="C25" s="3"/>
       <c r="D25" s="5"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="29"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="15"/>
     </row>
     <row r="26" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" s="7"/>
       <c r="C26" s="3"/>
       <c r="D26" s="5"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="29"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="15"/>
     </row>
     <row r="27" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" s="7"/>
       <c r="C27" s="3"/>
       <c r="D27" s="5"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="29"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="15"/>
     </row>
     <row r="28" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="7"/>
       <c r="C28" s="3"/>
       <c r="D28" s="5"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="29"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="15"/>
     </row>
     <row r="29" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="7"/>
       <c r="C29" s="3"/>
       <c r="D29" s="5"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="29"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="15"/>
     </row>
     <row r="30" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="7"/>
       <c r="C30" s="3"/>
       <c r="D30" s="5"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="29"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="15"/>
     </row>
     <row r="31" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="7"/>
       <c r="C31" s="3"/>
       <c r="D31" s="5"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="29"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="15"/>
     </row>
     <row r="32" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="7"/>
       <c r="C32" s="3"/>
       <c r="D32" s="5"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="29"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="15"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:G16">

</xml_diff>

<commit_message>
SCRUM-13 fin test lien JIRA
</commit_message>
<xml_diff>
--- a/gestion-projet/ProductBacklog.xlsx
+++ b/gestion-projet/ProductBacklog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wsjs\stacktrace\gestion-projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1EDAA95-EBE1-4DE2-8239-54AC602817ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37AFDBFA-CCE3-4697-B1F1-7F4F7BA732E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{1FDB83B7-599D-4D42-AA13-F5EE32DADB90}"/>
   </bookViews>
@@ -716,8 +716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52D07A81-0E55-45DE-A090-3CCE23AAB227}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -814,7 +814,7 @@
         <v>9</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="G6" s="22"/>
     </row>
@@ -835,7 +835,7 @@
         <v>9</v>
       </c>
       <c r="F7" s="21" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="G7" s="22"/>
     </row>
@@ -1197,6 +1197,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="c63466df-5bf8-40c0-9727-84c964796c6c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c1151b1f-6606-410d-809f-7631a57cef21">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010068EBBEFDE3F3A84D9AC5A24A258B13DB" ma:contentTypeVersion="11" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="edc10a4343b713180da3dec813c87c49">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c1151b1f-6606-410d-809f-7631a57cef21" xmlns:ns3="c63466df-5bf8-40c0-9727-84c964796c6c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c35e3451937de12e4696d094194e46ad" ns2:_="" ns3:_="">
     <xsd:import namespace="c1151b1f-6606-410d-809f-7631a57cef21"/>
@@ -1391,27 +1411,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="c63466df-5bf8-40c0-9727-84c964796c6c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c1151b1f-6606-410d-809f-7631a57cef21">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56DC5A8B-BDCE-424C-A578-1FE07D0F1105}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{856D492A-8E24-444B-90A6-CF668DEB4A9F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c63466df-5bf8-40c0-9727-84c964796c6c"/>
+    <ds:schemaRef ds:uri="c1151b1f-6606-410d-809f-7631a57cef21"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D32F45-18C1-42F1-811C-BA7793D4B09B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1428,23 +1447,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{856D492A-8E24-444B-90A6-CF668DEB4A9F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c63466df-5bf8-40c0-9727-84c964796c6c"/>
-    <ds:schemaRef ds:uri="c1151b1f-6606-410d-809f-7631a57cef21"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56DC5A8B-BDCE-424C-A578-1FE07D0F1105}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>